<commit_message>
Úprava souboru missing data overview.
</commit_message>
<xml_diff>
--- a/Missing_data_overview.xlsx
+++ b/Missing_data_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouck\Engeto\Data_academy\Covid19_SQL_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179D55DB-5443-4EB6-8F55-BA99EF6AD692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B235CDD9-1A55-4BCD-8FE5-42743AFF8538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4578DD4D-0619-4E3C-8429-8B929A177B4C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="176">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -556,13 +556,19 @@
   </si>
   <si>
     <t xml:space="preserve"> 81 states (43 %)</t>
+  </si>
+  <si>
+    <t>MISSING DATA OVERVIEW</t>
+  </si>
+  <si>
+    <t>For following states data are not available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +605,24 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -742,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -767,6 +791,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1082,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56FF542-90AE-45E1-8327-A0D893155FFE}">
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,878 +1130,860 @@
     <col min="9" max="9" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="I10" s="2" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="I11" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>143</v>
+        <v>61</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="G16" s="2" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>139</v>
+        <v>62</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1981,12 +1993,12 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1996,12 +2008,12 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2011,12 +2023,12 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2026,12 +2038,12 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2041,12 +2053,12 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2056,12 +2068,12 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2071,12 +2083,12 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2086,12 +2098,12 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2101,12 +2113,12 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2116,12 +2128,12 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2131,12 +2143,12 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2146,12 +2158,12 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2161,12 +2173,12 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2176,12 +2188,12 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2191,12 +2203,12 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2206,12 +2218,12 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2221,12 +2233,12 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2236,12 +2248,12 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2251,12 +2263,12 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2266,12 +2278,12 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2281,12 +2293,12 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2296,12 +2308,12 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2311,12 +2323,12 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2326,12 +2338,12 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2341,12 +2353,12 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2356,12 +2368,12 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2371,12 +2383,12 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2386,12 +2398,12 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2401,12 +2413,12 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2416,12 +2428,12 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2431,12 +2443,12 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2446,12 +2458,12 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2461,12 +2473,12 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2476,12 +2488,12 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2491,12 +2503,12 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2506,12 +2518,12 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2521,12 +2533,12 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2536,12 +2548,12 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2551,12 +2563,12 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2566,12 +2578,12 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2581,12 +2593,12 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2596,11 +2608,13 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
+      <c r="A84" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -2609,11 +2623,13 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2" t="s">
-        <v>46</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="3"/>
+      <c r="A85" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -2622,11 +2638,13 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="3"/>
+      <c r="A86" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -2635,7 +2653,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -2648,7 +2666,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -2661,7 +2679,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -2674,7 +2692,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
@@ -2687,7 +2705,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
@@ -2700,7 +2718,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -2713,7 +2731,7 @@
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -2726,7 +2744,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -2739,7 +2757,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -2752,7 +2770,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
@@ -2765,7 +2783,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -2778,7 +2796,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
@@ -2791,7 +2809,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -2804,7 +2822,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -2817,7 +2835,7 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -2830,7 +2848,7 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
@@ -2843,7 +2861,7 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
@@ -2856,7 +2874,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2" t="s">
-        <v>125</v>
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
@@ -2869,7 +2887,7 @@
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
@@ -2882,7 +2900,7 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2" t="s">
-        <v>127</v>
+        <v>57</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -2895,7 +2913,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
@@ -2908,7 +2926,7 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -2921,7 +2939,7 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
@@ -2934,7 +2952,7 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -2947,7 +2965,7 @@
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -2960,7 +2978,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -2973,7 +2991,7 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
@@ -2986,7 +3004,7 @@
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -2999,7 +3017,7 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
@@ -3012,7 +3030,7 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -3025,7 +3043,7 @@
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
       <c r="I116" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -3038,7 +3056,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -3051,7 +3069,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -3064,7 +3082,7 @@
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -3077,7 +3095,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -3090,7 +3108,7 @@
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -3103,7 +3121,7 @@
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -3116,7 +3134,7 @@
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
@@ -3129,7 +3147,7 @@
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
@@ -3142,7 +3160,7 @@
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
@@ -3155,7 +3173,7 @@
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -3168,7 +3186,7 @@
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
@@ -3181,7 +3199,7 @@
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
@@ -3194,7 +3212,7 @@
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -3207,7 +3225,7 @@
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
@@ -3220,7 +3238,7 @@
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -3233,7 +3251,7 @@
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -3246,7 +3264,7 @@
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
@@ -3259,7 +3277,7 @@
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
@@ -3272,7 +3290,7 @@
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
@@ -3285,7 +3303,7 @@
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
       <c r="I136" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
@@ -3298,7 +3316,7 @@
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
@@ -3311,7 +3329,7 @@
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
       <c r="I138" s="2" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
@@ -3324,7 +3342,7 @@
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -3337,7 +3355,7 @@
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
@@ -3350,7 +3368,7 @@
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
@@ -3363,7 +3381,7 @@
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
       <c r="I142" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
@@ -3376,7 +3394,7 @@
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
@@ -3389,7 +3407,7 @@
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
@@ -3402,7 +3420,7 @@
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
       <c r="I145" s="2" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
@@ -3415,7 +3433,7 @@
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
       <c r="I146" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
@@ -3428,7 +3446,7 @@
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
@@ -3441,7 +3459,7 @@
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
       <c r="I148" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
@@ -3454,7 +3472,7 @@
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
@@ -3467,7 +3485,7 @@
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
@@ -3480,7 +3498,7 @@
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
@@ -3493,7 +3511,7 @@
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
       <c r="I152" s="2" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
@@ -3506,7 +3524,7 @@
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
@@ -3519,7 +3537,7 @@
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
@@ -3532,7 +3550,7 @@
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
@@ -3545,7 +3563,7 @@
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
       <c r="I156" s="2" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -3558,23 +3576,66 @@
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
       <c r="I157" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" s="3"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" s="3"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" s="3"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="4"/>
-      <c r="B158" s="5"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="5"/>
-      <c r="E158" s="5"/>
-      <c r="F158" s="5"/>
-      <c r="G158" s="5"/>
-      <c r="H158" s="5"/>
-      <c r="I158" s="5" t="s">
+    <row r="161" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A161" s="4"/>
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="5" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>